<commit_message>
upload první stabilní verze pro nastavování ipv4 adres
</commit_message>
<xml_diff>
--- a/IP_setting/saved_adresses_2.xlsx
+++ b/IP_setting/saved_adresses_2.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
@@ -406,12 +406,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.100.241</t>
+          <t>192.168.100.2455</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Nonedafdaf</t>
         </is>
       </c>
     </row>
@@ -423,17 +428,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.100.241</t>
+          <t>192.168.100.244</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>gfh</t>
         </is>
       </c>
     </row>
@@ -478,28 +478,6 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>a</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.180.241</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>vcz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
vyreseno mounteni disku, vyhledavani, nastavovani oblibenych projektu, schovana maska, nova nastaveni,ktera se ukladaji po zavreni aplikace
</commit_message>
<xml_diff>
--- a/IP_setting/saved_adresses_2.xlsx
+++ b/IP_setting/saved_adresses_2.xlsx
@@ -3,10 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9600" yWindow="15" windowWidth="28800" windowHeight="15885" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ip_adress_list" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Favourite" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Settings" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -49,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -392,8 +394,8 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -401,12 +403,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>dfhghd</t>
+          <t>hgf</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.100.2455</t>
+          <t>192.168.100.244</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -416,36 +418,41 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Nonedafdaf</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>hgf</t>
+          <t>sgf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.100.244</t>
+          <t>192.168.100.241</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>sfg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sgf</t>
+          <t>dfhghd</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.100.241</t>
+          <t>192.168.100.2455</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -455,7 +462,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sfg</t>
+          <t>Nonedafdaf</t>
         </is>
       </c>
     </row>
@@ -477,7 +484,91 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>a
+d
+hgfghd
+d</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>hgf</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>192.168.100.244</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="48.5703125" customWidth="1" min="1" max="1"/>
+    <col width="71.7109375" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nastavení default rozhraní pro editaci IP adresy</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>list názvů rozhraní</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ethernet,Ethernet1,Ethernet2,Ethernet3,Ethernet4,Ethernet5,Wi-Fi,USB_Ethernet</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upload nové verze ip setting, oprava chyb, nový způsob vizualizace
</commit_message>
<xml_diff>
--- a/IP_setting/saved_adresses_2.xlsx
+++ b/IP_setting/saved_adresses_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9600" yWindow="15" windowWidth="28800" windowHeight="15885" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_adress_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -392,10 +392,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:D2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -403,12 +403,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>hgf</t>
+          <t>sgf</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.100.244</t>
+          <t>192.168.100.241</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -418,14 +418,14 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>sfg</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sgf</t>
+          <t>514</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -440,19 +440,21 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sfg</t>
+          <t>afs
+asdf
+asdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dfhghd</t>
+          <t>sfdgsfg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.100.2455</t>
+          <t>192.168.100.241</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -462,19 +464,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nonedafdaf</t>
+          <t>sfs</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>dsf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.14.241</t>
+          <t>192.168.100.241</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -484,10 +486,29 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>a
-d
-hgfghd
-d</t>
+          <t>fffffffffffffffffffffffffffffff</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sf</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.100.241</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sdfsfdddddddddddddd</t>
         </is>
       </c>
     </row>
@@ -541,7 +562,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>